<commit_message>
added results of ksom wallfollow best hps
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_wallFollow_01_hold_02_best.xlsx
+++ b/results_analysis/ksom_wallFollow_01_hold_02_best.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp2\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D99B22A-20B3-4468-A9AC-1F1D11FC3874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB020A8-F34C-4FD8-B34E-DC8E9E6F8A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_hp_best" sheetId="1" r:id="rId1"/>
@@ -105,18 +105,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -449,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,12 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,13 +509,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -559,41 +572,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A889A0D-6079-4851-A2AA-AD4BB1CBB64D}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -985,29 +965,29 @@
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="33">
-        <v>0.62026431718061703</v>
-      </c>
-      <c r="D3" s="33">
-        <v>0.79383259911894299</v>
-      </c>
-      <c r="E3" s="33">
-        <v>0.79361233480176196</v>
-      </c>
-      <c r="F3" s="33">
-        <v>0.78788546255506597</v>
-      </c>
-      <c r="G3" s="33">
-        <v>0.79537444933920698</v>
-      </c>
-      <c r="H3" s="33">
-        <v>0.79515418502202595</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0.80726872246696002</v>
-      </c>
-      <c r="J3" s="34">
-        <v>0.808810572687225</v>
+      <c r="C3" s="25">
+        <v>0.75352422907489003</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.80528634361233498</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.81101321585903097</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.80572687224669604</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.80837004405286295</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.81057268722467002</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.804625550660793</v>
+      </c>
+      <c r="J3" s="26">
+        <v>0.81497797356828205</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1015,29 +995,29 @@
       <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35">
-        <v>0.61277533039647603</v>
-      </c>
-      <c r="D4" s="35">
-        <v>0.62246696035242299</v>
-      </c>
-      <c r="E4" s="35">
-        <v>0.61409691629955898</v>
-      </c>
-      <c r="F4" s="35">
-        <v>0.78590308370044104</v>
-      </c>
-      <c r="G4" s="35">
-        <v>0.82665198237885495</v>
-      </c>
-      <c r="H4" s="35">
-        <v>0.79977973568281902</v>
-      </c>
-      <c r="I4" s="35">
-        <v>0.60837004405286299</v>
-      </c>
-      <c r="J4" s="36">
-        <v>0.61167400881057299</v>
+      <c r="C4" s="27">
+        <v>0.73303964757709295</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.82577092511013195</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.61563876651982397</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0.78193832599118895</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0.80264317180616696</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0.80374449339206999</v>
+      </c>
+      <c r="I4" s="27">
+        <v>0.61607929515418502</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0.76453744493392095</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1045,29 +1025,29 @@
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35">
-        <v>0.74911894273127799</v>
-      </c>
-      <c r="D5" s="35">
-        <v>0.80220264317180601</v>
-      </c>
-      <c r="E5" s="35">
-        <v>0.79735682819383302</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0.79933920704845796</v>
-      </c>
-      <c r="G5" s="35">
+      <c r="C5" s="27">
+        <v>0.75837004405286401</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.81607929515418498</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.81013215859030796</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.79691629955947096</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0.81365638766519799</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0.81189427312775297</v>
+      </c>
+      <c r="I5" s="27">
         <v>0.81145374449339203</v>
       </c>
-      <c r="H5" s="35">
-        <v>0.81079295154185005</v>
-      </c>
-      <c r="I5" s="35">
-        <v>0.79845814977973595</v>
-      </c>
-      <c r="J5" s="36">
-        <v>0.82863436123348</v>
+      <c r="J5" s="28">
+        <v>0.83237885462555095</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1077,29 +1057,29 @@
       <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35">
-        <v>0.61696035242290803</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0.79735682819383302</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0.790528634361233</v>
-      </c>
-      <c r="F6" s="35">
-        <v>0.79757709251101305</v>
-      </c>
-      <c r="G6" s="35">
-        <v>0.77973568281938299</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0.81057268722467002</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0.8</v>
-      </c>
-      <c r="J6" s="36">
-        <v>0.798017621145374</v>
+      <c r="C6" s="27">
+        <v>0.75176211453744501</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.75903083700440499</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.777312775330396</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.63215859030836996</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.76255506607929502</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0.75044052863436095</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0.76035242290748895</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0.63480176211453698</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1107,29 +1087,29 @@
       <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35">
-        <v>0.73920704845815</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.66872246696035198</v>
-      </c>
-      <c r="E7" s="35">
-        <v>0.61409691629955898</v>
-      </c>
-      <c r="F7" s="35">
-        <v>0.78546255506607898</v>
-      </c>
-      <c r="G7" s="35">
-        <v>0.610132158590308</v>
-      </c>
-      <c r="H7" s="35">
-        <v>0.60638766519823795</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0.72290748898678403</v>
-      </c>
-      <c r="J7" s="36">
-        <v>0.61740088105726898</v>
+      <c r="C7" s="27">
+        <v>0.75550660792951496</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.753303964757709</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.74185022026431702</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.73568281938325997</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.756607929515419</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.74713656387665195</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.75044052863436095</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0.764096916299559</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1137,29 +1117,29 @@
       <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="37">
-        <v>0.736784140969163</v>
-      </c>
-      <c r="D8" s="37">
-        <v>0.80176211453744495</v>
-      </c>
-      <c r="E8" s="37">
-        <v>0.80154185022026403</v>
-      </c>
-      <c r="F8" s="37">
-        <v>0.788105726872247</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.80044052863436099</v>
-      </c>
-      <c r="H8" s="37">
-        <v>0.78876651982378898</v>
-      </c>
-      <c r="I8" s="37">
-        <v>0.79030837004405297</v>
-      </c>
-      <c r="J8" s="38">
-        <v>0.79295154185021999</v>
+      <c r="C8" s="29">
+        <v>0.76982378854625599</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.75286343612334805</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0.75352422907489003</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0.76101321585903103</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0.75616740088105705</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.77621145374449296</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.75066079295154198</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0.76828193832599101</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1170,74 +1150,74 @@
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="30" t="s">
+      <c r="K11" s="38"/>
+      <c r="L11" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="31"/>
-      <c r="N11" s="30" t="s">
+      <c r="M11" s="38"/>
+      <c r="N11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="32"/>
+      <c r="O11" s="39"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1248,40 +1228,40 @@
       <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="34">
         <v>1.5625E-2</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <v>32</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="19">
         <v>256</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="19">
         <v>1</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="19">
         <v>1024</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="19">
         <v>32</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="19">
         <v>32</v>
       </c>
-      <c r="L13" s="39">
+      <c r="L13" s="31">
         <v>1.953125E-3</v>
       </c>
-      <c r="M13" s="39">
+      <c r="M13" s="31">
         <v>7.8125E-3</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="19">
         <v>256</v>
       </c>
       <c r="O13" s="4">
@@ -1293,43 +1273,43 @@
       <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="20">
         <v>512</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="21">
         <v>0.5</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="21">
         <v>4</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="21">
         <v>64</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="21">
         <v>0.4</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="21">
         <v>32</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="21">
         <v>1</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="21">
         <v>0.8</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="21">
         <v>32</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="32">
         <v>7.8125E-3</v>
       </c>
-      <c r="M14" s="40">
+      <c r="M14" s="32">
         <v>3.90625E-3</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="21">
         <v>1</v>
       </c>
-      <c r="O14" s="24">
+      <c r="O14" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1338,43 +1318,43 @@
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="35">
         <v>3.125E-2</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="21">
         <v>16</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="21">
         <v>0.5</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="21">
         <v>512</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="21">
         <v>0.4</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="21">
         <v>8</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="21">
         <v>16</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="21">
         <v>2.6</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="21">
         <v>16</v>
       </c>
-      <c r="L15" s="40">
+      <c r="L15" s="32">
         <v>9.765625E-4</v>
       </c>
-      <c r="M15" s="40">
+      <c r="M15" s="32">
         <v>-3.125E-2</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="21">
         <v>2</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1385,43 +1365,43 @@
       <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="35">
         <v>3.125E-2</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="21">
         <v>32</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="32">
         <v>7.8125E-3</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="21">
         <v>64</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="21">
         <v>0.8</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="21">
         <v>1</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="21">
         <v>32</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="21">
         <v>2.6</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="21">
         <v>32</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16" s="32">
         <v>1.953125E-3</v>
       </c>
-      <c r="M16" s="40">
+      <c r="M16" s="32">
         <v>9.765625E-4</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="21">
         <v>16</v>
       </c>
-      <c r="O16" s="24">
+      <c r="O16" s="22">
         <v>32</v>
       </c>
     </row>
@@ -1430,43 +1410,43 @@
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="20">
         <v>1024</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="21">
         <v>0.5</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="21">
         <v>0.125</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="21">
         <v>32</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="21">
         <v>1</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="21">
         <v>256</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="21">
         <v>16</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="21">
         <v>0.8</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="21">
         <v>2</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="21">
         <v>0.25</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="21">
         <v>1</v>
       </c>
-      <c r="N17" s="40">
+      <c r="N17" s="32">
         <v>3.90625E-3</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17" s="22">
         <v>0.5</v>
       </c>
     </row>
@@ -1475,43 +1455,43 @@
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="36">
         <v>1.953125E-3</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="23">
         <v>8</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="33">
         <v>1.953125E-3</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="23">
         <v>1</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="23">
         <v>1</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="23">
         <v>1024</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="23">
         <v>32</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="23">
         <v>2</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="23">
         <v>32</v>
       </c>
-      <c r="L18" s="41">
+      <c r="L18" s="33">
         <v>9.765625E-4</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="23">
         <v>0.5</v>
       </c>
-      <c r="N18" s="41">
+      <c r="N18" s="33">
         <v>1.953125E-3</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="24">
         <v>16</v>
       </c>
     </row>
@@ -1530,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1575,187 +1555,187 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="33">
-        <v>0.60354625550660801</v>
-      </c>
-      <c r="D3" s="33">
-        <v>0.70400881057268705</v>
-      </c>
-      <c r="E3" s="33">
-        <v>0.66273127753303995</v>
-      </c>
-      <c r="F3" s="33">
-        <v>0.69662995594713695</v>
-      </c>
-      <c r="G3" s="33">
-        <v>0.69557268722467003</v>
-      </c>
-      <c r="H3" s="27">
-        <v>0.71819383259911895</v>
-      </c>
-      <c r="I3" s="27">
-        <v>0.73255506607929499</v>
-      </c>
-      <c r="J3" s="28">
-        <v>0.73321585903083697</v>
+      <c r="C3" s="40">
+        <v>0.60968502202643204</v>
+      </c>
+      <c r="D3" s="40">
+        <v>0.77968942731277502</v>
+      </c>
+      <c r="E3" s="40">
+        <v>0.77281718061673998</v>
+      </c>
+      <c r="F3" s="40">
+        <v>0.76540748898678401</v>
+      </c>
+      <c r="G3" s="40">
+        <v>0.77552202643171797</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0.77419162995594704</v>
+      </c>
+      <c r="I3" s="40">
+        <v>0.77800660792951604</v>
+      </c>
+      <c r="J3" s="41">
+        <v>0.77146916299559498</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35">
-        <v>0.42028634361233502</v>
-      </c>
-      <c r="D4" s="35">
-        <v>0.45640969162995598</v>
-      </c>
-      <c r="E4" s="35">
-        <v>0.39442731277533</v>
-      </c>
-      <c r="F4" s="15">
-        <v>0.66383259911894299</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.53801762114537399</v>
-      </c>
-      <c r="H4" s="15">
-        <v>0.58088105726872197</v>
-      </c>
-      <c r="I4" s="35">
-        <v>0.49696035242290798</v>
-      </c>
-      <c r="J4" s="36">
-        <v>0.475594713656388</v>
+      <c r="C4" s="42">
+        <v>0.49537665198237901</v>
+      </c>
+      <c r="D4" s="42">
+        <v>0.53148678414096895</v>
+      </c>
+      <c r="E4" s="42">
+        <v>0.47322687224669602</v>
+      </c>
+      <c r="F4" s="42">
+        <v>0.60663215859030795</v>
+      </c>
+      <c r="G4" s="42">
+        <v>0.51273788546255505</v>
+      </c>
+      <c r="H4" s="42">
+        <v>0.51921365638766503</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0.43001762114537401</v>
+      </c>
+      <c r="J4" s="43">
+        <v>0.50853964757709302</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35">
-        <v>0.58273127753303999</v>
-      </c>
-      <c r="D5" s="35">
-        <v>0.72253303964757698</v>
-      </c>
-      <c r="E5" s="15">
-        <v>0.75160792951541899</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0.73191629955947102</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.76182819383259903</v>
-      </c>
-      <c r="H5" s="15">
-        <v>0.750814977973568</v>
-      </c>
-      <c r="I5" s="15">
-        <v>0.75107929515418503</v>
-      </c>
-      <c r="J5" s="36">
-        <v>0.74870044052863405</v>
+      <c r="C5" s="42">
+        <v>0.58631497797356802</v>
+      </c>
+      <c r="D5" s="42">
+        <v>0.76479955947136602</v>
+      </c>
+      <c r="E5" s="42">
+        <v>0.76504405286343602</v>
+      </c>
+      <c r="F5" s="42">
+        <v>0.70205947136563895</v>
+      </c>
+      <c r="G5" s="42">
+        <v>0.75740528634361204</v>
+      </c>
+      <c r="H5" s="42">
+        <v>0.753162995594714</v>
+      </c>
+      <c r="I5" s="42">
+        <v>0.78784801762114498</v>
+      </c>
+      <c r="J5" s="43">
+        <v>0.603665198237885</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35">
-        <v>0.600132158590308</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0.704493392070485</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.75149779735682798</v>
-      </c>
-      <c r="F6" s="35">
-        <v>0.67484581497797402</v>
-      </c>
-      <c r="G6" s="15">
-        <v>0.72259911894273099</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0.71737885462555095</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0.70819383259911906</v>
-      </c>
-      <c r="J6" s="29">
-        <v>0.74707048458149805</v>
+      <c r="C6" s="42">
+        <v>0.60774229074889896</v>
+      </c>
+      <c r="D6" s="42">
+        <v>0.60589867841409695</v>
+      </c>
+      <c r="E6" s="42">
+        <v>0.60850220264317201</v>
+      </c>
+      <c r="F6" s="42">
+        <v>0.60886784140969197</v>
+      </c>
+      <c r="G6" s="42">
+        <v>0.60683259911894305</v>
+      </c>
+      <c r="H6" s="42">
+        <v>0.60707709251101305</v>
+      </c>
+      <c r="I6" s="42">
+        <v>0.60851982378854597</v>
+      </c>
+      <c r="J6" s="43">
+        <v>0.60542731277533102</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="47"/>
-      <c r="B7" s="48" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35">
-        <v>0.48066079295154202</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.46651982378854601</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0.49903083700440498</v>
-      </c>
-      <c r="F7" s="15">
-        <v>0.673039647577093</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0.51165198237885501</v>
-      </c>
-      <c r="H7" s="35">
-        <v>0.41129955947136598</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0.48790748898678399</v>
-      </c>
-      <c r="J7" s="36">
-        <v>0.44079295154185</v>
+      <c r="C7" s="42">
+        <v>0.48772466960352401</v>
+      </c>
+      <c r="D7" s="42">
+        <v>0.48175330396475802</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0.46383039647577101</v>
+      </c>
+      <c r="F7" s="42">
+        <v>0.51148678414096904</v>
+      </c>
+      <c r="G7" s="42">
+        <v>0.46964537444933901</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0.48463436123348003</v>
+      </c>
+      <c r="I7" s="42">
+        <v>0.479909691629956</v>
+      </c>
+      <c r="J7" s="43">
+        <v>0.50255286343612304</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="46"/>
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="37">
-        <v>0.49343612334801801</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0.78266519823788505</v>
-      </c>
-      <c r="E8" s="16">
-        <v>0.76174008810572702</v>
-      </c>
-      <c r="F8" s="37">
-        <v>0.69215859030837001</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.71541850220264303</v>
-      </c>
-      <c r="H8" s="37">
-        <v>0.72156387665198196</v>
-      </c>
-      <c r="I8" s="16">
-        <v>0.75812775330396498</v>
-      </c>
-      <c r="J8" s="38">
-        <v>0.75229074889867797</v>
+      <c r="C8" s="44">
+        <v>0.52212334801762095</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0.57534581497797399</v>
+      </c>
+      <c r="E8" s="44">
+        <v>0.559011013215859</v>
+      </c>
+      <c r="F8" s="44">
+        <v>0.56632819383259903</v>
+      </c>
+      <c r="G8" s="44">
+        <v>0.52394273127753299</v>
+      </c>
+      <c r="H8" s="44">
+        <v>0.57229295154185</v>
+      </c>
+      <c r="I8" s="44">
+        <v>0.58250220264317198</v>
+      </c>
+      <c r="J8" s="45">
+        <v>0.553077092511013</v>
       </c>
     </row>
   </sheetData>
@@ -1817,29 +1797,29 @@
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="33">
-        <v>0.61101321585903101</v>
-      </c>
-      <c r="D3" s="33">
-        <v>0.74988986784140998</v>
-      </c>
-      <c r="E3" s="33">
-        <v>0.74129955947136605</v>
-      </c>
-      <c r="F3" s="33">
-        <v>0.69129955947136601</v>
-      </c>
-      <c r="G3" s="33">
-        <v>0.72378854625550704</v>
-      </c>
-      <c r="H3" s="33">
-        <v>0.73634361233480194</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0.78160792951541902</v>
-      </c>
-      <c r="J3" s="34">
-        <v>0.75308370044052897</v>
+      <c r="C3" s="25">
+        <v>0.60969162995594695</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.78909691629956003</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.78149779735682801</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.784801762114537</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.783920704845815</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.78270925110132195</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.78678414096916305</v>
+      </c>
+      <c r="J3" s="26">
+        <v>0.78116740088105696</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1847,29 +1827,29 @@
       <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35">
-        <v>0.34878854625550698</v>
-      </c>
-      <c r="D4" s="35">
-        <v>0.46002202643171802</v>
-      </c>
-      <c r="E4" s="35">
-        <v>0.33083700440528602</v>
-      </c>
-      <c r="F4" s="35">
-        <v>0.66541850220264298</v>
-      </c>
-      <c r="G4" s="35">
-        <v>0.51310572687224698</v>
-      </c>
-      <c r="H4" s="35">
-        <v>0.61079295154184998</v>
-      </c>
-      <c r="I4" s="35">
-        <v>0.53248898678414103</v>
-      </c>
-      <c r="J4" s="36">
-        <v>0.55517621145374396</v>
+      <c r="C4" s="27">
+        <v>0.48149779735682802</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.54284140969162997</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.36971365638766501</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0.61266519823788601</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0.54328193832599103</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0.46971365638766499</v>
+      </c>
+      <c r="I4" s="27">
+        <v>0.35825991189427298</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0.54063876651982401</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1877,29 +1857,29 @@
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35">
-        <v>0.60781938325991203</v>
-      </c>
-      <c r="D5" s="35">
-        <v>0.74526431718061703</v>
-      </c>
-      <c r="E5" s="35">
-        <v>0.76167400881057301</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0.77037444933920696</v>
-      </c>
-      <c r="G5" s="35">
-        <v>0.75770925110132203</v>
-      </c>
-      <c r="H5" s="35">
-        <v>0.78017621145374505</v>
-      </c>
-      <c r="I5" s="35">
-        <v>0.77433920704845804</v>
-      </c>
-      <c r="J5" s="36">
-        <v>0.77444933920704795</v>
+      <c r="C5" s="27">
+        <v>0.61629955947136605</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.76354625550660804</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.75638766519823797</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.743392070484581</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0.74856828193832603</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0.74647577092510997</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.78909691629956003</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0.60704845814978003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1909,29 +1889,29 @@
       <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35">
-        <v>0.60748898678414098</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0.70914096916299596</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0.77808370044052899</v>
-      </c>
-      <c r="F6" s="35">
-        <v>0.62323788546255499</v>
-      </c>
-      <c r="G6" s="35">
-        <v>0.772356828193833</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0.77037444933920696</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0.75143171806167397</v>
-      </c>
-      <c r="J6" s="36">
-        <v>0.77709251101321597</v>
+      <c r="C6" s="27">
+        <v>0.61101321585903101</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.61068281938325997</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.61167400881057299</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.610903083700441</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.61079295154184998</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0.61035242290748903</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0.60991189427312797</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0.61057268722466995</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1939,29 +1919,29 @@
       <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35">
-        <v>0.41949339207048503</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.50253303964757701</v>
-      </c>
-      <c r="E7" s="35">
-        <v>0.52577092511013201</v>
-      </c>
-      <c r="F7" s="35">
-        <v>0.706938325991189</v>
-      </c>
-      <c r="G7" s="35">
-        <v>0.60484581497797396</v>
-      </c>
-      <c r="H7" s="35">
-        <v>0.45605726872246699</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0.46751101321585897</v>
-      </c>
-      <c r="J7" s="36">
-        <v>0.45</v>
+      <c r="C7" s="27">
+        <v>0.455726872246696</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.45363436123348</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.45308370044052898</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.54955947136563899</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.45330396475770901</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.45550660792951497</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.45440528634361199</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0.45638766519823798</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1969,29 +1949,29 @@
       <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="37">
-        <v>0.452422907488987</v>
-      </c>
-      <c r="D8" s="37">
-        <v>0.79449339207048497</v>
-      </c>
-      <c r="E8" s="37">
-        <v>0.78259911894273104</v>
-      </c>
-      <c r="F8" s="37">
-        <v>0.67235682819383302</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.75781938325991205</v>
-      </c>
-      <c r="H8" s="37">
-        <v>0.76101321585903103</v>
-      </c>
-      <c r="I8" s="37">
-        <v>0.76508810572687203</v>
-      </c>
-      <c r="J8" s="38">
-        <v>0.75892070484581498</v>
+      <c r="C8" s="29">
+        <v>0.45462555066079302</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.61035242290748903</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0.60837004405286299</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0.60914096916299598</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0.45550660792951497</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.61145374449339196</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.60947136563876703</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0.59361233480176201</v>
       </c>
     </row>
   </sheetData>
@@ -2053,29 +2033,29 @@
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="33">
-        <v>0.61886764094957802</v>
-      </c>
-      <c r="D3" s="33">
-        <v>0.766643748569942</v>
-      </c>
-      <c r="E3" s="33">
-        <v>0.76160647932622405</v>
-      </c>
-      <c r="F3" s="33">
-        <v>0.74307472086943305</v>
-      </c>
-      <c r="G3" s="33">
-        <v>0.75952790098161405</v>
-      </c>
-      <c r="H3" s="33">
-        <v>0.76766595567255402</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0.78015663317693795</v>
-      </c>
-      <c r="J3" s="34">
-        <v>0.772899779649726</v>
+      <c r="C3" s="25">
+        <v>0.72039622404238901</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.77945979850376701</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.78328461938654403</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.77107403843088496</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.78070145093117904</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.78143686689847203</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.77711911586105398</v>
+      </c>
+      <c r="J3" s="26">
+        <v>0.78069480772639499</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2083,29 +2063,29 @@
       <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35">
-        <v>0.60593089556964796</v>
-      </c>
-      <c r="D4" s="35">
-        <v>0.539743373789491</v>
-      </c>
-      <c r="E4" s="35">
-        <v>0.61141819401573405</v>
-      </c>
-      <c r="F4" s="35">
-        <v>0.75846315025511502</v>
-      </c>
-      <c r="G4" s="35">
-        <v>0.78472907446790996</v>
-      </c>
-      <c r="H4" s="35">
-        <v>0.75421215686387399</v>
-      </c>
-      <c r="I4" s="35">
-        <v>0.60632914717966302</v>
-      </c>
-      <c r="J4" s="36">
-        <v>0.60526864013858905</v>
+      <c r="C4" s="27">
+        <v>0.59798872917264301</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.78606731867824498</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.611736789270656</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0.74496955183081803</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0.75422936311298705</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0.77039714090852096</v>
+      </c>
+      <c r="I4" s="27">
+        <v>0.61137995514800803</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0.60944182571554595</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2113,29 +2093,29 @@
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35">
-        <v>0.62174888042751197</v>
-      </c>
-      <c r="D5" s="35">
-        <v>0.76713222673674397</v>
-      </c>
-      <c r="E5" s="35">
-        <v>0.76417245023257696</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0.76967354833594204</v>
-      </c>
-      <c r="G5" s="35">
-        <v>0.78307854354320405</v>
-      </c>
-      <c r="H5" s="35">
-        <v>0.76945083229450295</v>
-      </c>
-      <c r="I5" s="35">
-        <v>0.76266274009255397</v>
-      </c>
-      <c r="J5" s="36">
-        <v>0.65283217859920495</v>
+      <c r="C5" s="27">
+        <v>0.61754564299216297</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.64133264599404505</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.77313107009787196</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.76070041431226498</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0.65550679550550095</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0.78348240136780201</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.64267477229109804</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0.80836342396848204</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2145,29 +2125,29 @@
       <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35">
-        <v>0.619863623631696</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0.76063086606805896</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0.76301854227561094</v>
-      </c>
-      <c r="F6" s="35">
-        <v>0.77477806775574298</v>
-      </c>
-      <c r="G6" s="35">
-        <v>0.74882092124532296</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0.78730747151664404</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0.77311089997151905</v>
-      </c>
-      <c r="J6" s="36">
-        <v>0.76437299232675704</v>
+      <c r="C6" s="27">
+        <v>0.70720322855220297</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.71783530829589204</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.74913657748302698</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.63460752601241199</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.74499783482306603</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0.69455673641559801</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0.71555053053632001</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0.64126099848797502</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2175,29 +2155,29 @@
       <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35">
-        <v>0.61728538524973897</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.61042471849954405</v>
-      </c>
-      <c r="E7" s="35">
-        <v>0.61124443238812398</v>
-      </c>
-      <c r="F7" s="35">
-        <v>0.75325503154455298</v>
-      </c>
-      <c r="G7" s="35">
-        <v>0.61379009126050699</v>
-      </c>
-      <c r="H7" s="35">
-        <v>0.60180026270551301</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0.71028586246543701</v>
-      </c>
-      <c r="J7" s="36">
-        <v>0.61783454315483799</v>
+      <c r="C7" s="27">
+        <v>0.61314872136518395</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.61146545774876804</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.60224976089358395</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.59619186370807997</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.60821083079189298</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.60070195234958002</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.61522451073358697</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0.62916997976008004</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2205,29 +2185,29 @@
       <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="37">
-        <v>0.60062878804722397</v>
-      </c>
-      <c r="D8" s="37">
-        <v>0.75321658362702404</v>
-      </c>
-      <c r="E8" s="37">
-        <v>0.76846313558534196</v>
-      </c>
-      <c r="F8" s="37">
-        <v>0.75539295687233599</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.771269192420037</v>
-      </c>
-      <c r="H8" s="37">
-        <v>0.75770038564748599</v>
-      </c>
-      <c r="I8" s="37">
-        <v>0.75649659613539699</v>
-      </c>
-      <c r="J8" s="38">
-        <v>0.76677162348467798</v>
+      <c r="C8" s="29">
+        <v>0.62326313868963601</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.62100689088692396</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0.61859082818961797</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0.71677274165608396</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0.61352000849389698</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.62428389599225598</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.62544528860359805</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0.74171085257513003</v>
       </c>
     </row>
   </sheetData>
@@ -2289,29 +2269,29 @@
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="33">
-        <v>0.48580999890915899</v>
-      </c>
-      <c r="D3" s="33">
-        <v>0.68500200100675102</v>
-      </c>
-      <c r="E3" s="33">
-        <v>0.69230187092655004</v>
-      </c>
-      <c r="F3" s="33">
-        <v>0.67301455209619399</v>
-      </c>
-      <c r="G3" s="33">
-        <v>0.68834750372521702</v>
-      </c>
-      <c r="H3" s="33">
-        <v>0.68418168671860602</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0.70778451075415505</v>
-      </c>
-      <c r="J3" s="34">
-        <v>0.70775403149117599</v>
+      <c r="C3" s="25">
+        <v>0.63854095207524697</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.70010164499657501</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.71456381973252803</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.69781972581515195</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.70574414708656696</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.71095714072967897</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.70002815735457702</v>
+      </c>
+      <c r="J3" s="26">
+        <v>0.71957827950853503</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2319,29 +2299,29 @@
       <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35">
-        <v>0.48479263013877699</v>
-      </c>
-      <c r="D4" s="35">
-        <v>0.51919973072791503</v>
-      </c>
-      <c r="E4" s="35">
-        <v>0.48122643422517603</v>
-      </c>
-      <c r="F4" s="35">
-        <v>0.67041110475305299</v>
-      </c>
-      <c r="G4" s="35">
-        <v>0.72956080513936705</v>
-      </c>
-      <c r="H4" s="35">
-        <v>0.69647899731268004</v>
-      </c>
-      <c r="I4" s="35">
-        <v>0.47975460890099197</v>
-      </c>
-      <c r="J4" s="36">
-        <v>0.48834435737343901</v>
+      <c r="C4" s="27">
+        <v>0.56566804686085004</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.72555707363910205</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.48438960861402602</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0.66063116276377798</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0.68456432089355801</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0.70329187314470398</v>
+      </c>
+      <c r="I4" s="27">
+        <v>0.48631300669919802</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0.61560850257572497</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2349,29 +2329,29 @@
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35">
-        <v>0.59065411871507101</v>
-      </c>
-      <c r="D5" s="35">
-        <v>0.69778377207819298</v>
-      </c>
-      <c r="E5" s="35">
-        <v>0.68900548681965201</v>
-      </c>
-      <c r="F5" s="35">
-        <v>0.68601717688018504</v>
-      </c>
-      <c r="G5" s="35">
-        <v>0.71725586335157598</v>
-      </c>
-      <c r="H5" s="35">
-        <v>0.71292995212451304</v>
-      </c>
-      <c r="I5" s="35">
-        <v>0.69056466545844597</v>
-      </c>
-      <c r="J5" s="36">
-        <v>0.72745735435564096</v>
+      <c r="C5" s="27">
+        <v>0.60574045008789001</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.70484902162723095</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.70904910980150404</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.68147035891282104</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0.70026989662205297</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0.71552493584032695</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.69603850098367803</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0.73834863580003196</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2381,29 +2361,29 @@
       <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35">
-        <v>0.50124484528207003</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0.69189791717859594</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0.68247669093874697</v>
-      </c>
-      <c r="F6" s="35">
-        <v>0.68883082028420795</v>
-      </c>
-      <c r="G6" s="35">
-        <v>0.656087924944323</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0.70938399137240205</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0.69423012215336599</v>
-      </c>
-      <c r="J6" s="36">
-        <v>0.68855070198414003</v>
+      <c r="C6" s="27">
+        <v>0.60761806839973398</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.62113700155858798</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.65130895497890795</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.51642277473200804</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.65370460754764603</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0.60657816222457595</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0.62091075481490698</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0.51937597439937599</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2411,29 +2391,29 @@
       <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35">
-        <v>0.57470532171149802</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.483094263955964</v>
-      </c>
-      <c r="E7" s="35">
-        <v>0.48586027877848498</v>
-      </c>
-      <c r="F7" s="35">
-        <v>0.67163930388955995</v>
-      </c>
-      <c r="G7" s="35">
-        <v>0.480498200613517</v>
-      </c>
-      <c r="H7" s="35">
-        <v>0.46741460663216799</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0.60938883221676898</v>
-      </c>
-      <c r="J7" s="36">
-        <v>0.49720869947588098</v>
+      <c r="C7" s="27">
+        <v>0.60094977607002698</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.59730325098800596</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.57929869963114999</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.56973421652396905</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.60245442540891203</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.58702988430775405</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.59288707254563899</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0.61492514221426897</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2441,29 +2421,29 @@
       <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="37">
-        <v>0.571435611618485</v>
-      </c>
-      <c r="D8" s="37">
-        <v>0.69559103837853398</v>
-      </c>
-      <c r="E8" s="37">
-        <v>0.70259114591268002</v>
-      </c>
-      <c r="F8" s="37">
-        <v>0.67435462464852003</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.69585210187350299</v>
-      </c>
-      <c r="H8" s="37">
-        <v>0.66983343065960899</v>
-      </c>
-      <c r="I8" s="37">
-        <v>0.67872187292478903</v>
-      </c>
-      <c r="J8" s="38">
-        <v>0.68261786230088795</v>
+      <c r="C8" s="29">
+        <v>0.62466946231800502</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.59729188519642396</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0.59751516098500301</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0.62187803489251103</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0.60211121507797805</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.63523903969254403</v>
+      </c>
+      <c r="I8" s="29">
+        <v>0.59325812352371998</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0.64018629477590006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>